<commit_message>
[user-app] Context API 테스트 코드 추가
</commit_message>
<xml_diff>
--- a/0 _ docs/0 _ db 설계.xlsx
+++ b/0 _ docs/0 _ db 설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev-ezen\rental-cars\0 _ docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C93532-08C6-4364-80A9-4529469BB802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AA1031-992A-43CE-80B5-45DF8D37D534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="975" windowWidth="14130" windowHeight="12045" xr2:uid="{27D1F9A5-D906-4A19-AD47-54230B13E495}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{27D1F9A5-D906-4A19-AD47-54230B13E495}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="113">
   <si>
     <t>customers (고객 정보)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -122,10 +122,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>desc</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>차량 ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -474,15 +470,23 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DB 설계 (최종 수정: 2024.02.05.MON 11:30:00)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>(0) 운행 전, (1) 운행 중, (2) 운행 종료</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>sso_login은 일단 false 설정</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pl_desc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>v_desc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB 설계 (최종 수정: 2024.02.15.THU 12:15:00)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -601,7 +605,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -641,6 +645,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,7 +749,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -880,6 +890,9 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1203,7 +1216,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98531398-C03B-4527-8006-CCEE9F94C8A2}">
   <dimension ref="C2:BF52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1213,7 +1228,7 @@
     <row r="2" spans="3:58" ht="14.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:58" ht="26.25" x14ac:dyDescent="0.3">
       <c r="C3" s="44" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
@@ -1300,7 +1315,7 @@
       <c r="S6" s="7"/>
       <c r="T6" s="8"/>
       <c r="W6" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="X6" s="13"/>
       <c r="Y6" s="13"/>
@@ -1318,7 +1333,7 @@
       <c r="AK6" s="13"/>
       <c r="AL6" s="14"/>
       <c r="AO6" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AP6" s="13"/>
       <c r="AQ6" s="13"/>
@@ -1391,7 +1406,7 @@
       <c r="AL8" s="21"/>
       <c r="AO8" s="24"/>
       <c r="AP8" s="27" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AQ8" s="27"/>
       <c r="AR8" s="27"/>
@@ -1402,7 +1417,7 @@
       <c r="AW8" s="27"/>
       <c r="AX8" s="27"/>
       <c r="AY8" s="27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AZ8" s="27"/>
       <c r="BA8" s="27"/>
@@ -1447,18 +1462,18 @@
       <c r="T10" s="3"/>
       <c r="W10" s="2"/>
       <c r="X10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="AG10" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="AL10" s="3"/>
       <c r="AO10" s="2"/>
       <c r="AP10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AY10" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="AY10" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="BD10" s="3"/>
       <c r="BF10" s="3"/>
@@ -1467,10 +1482,10 @@
       <c r="C11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="T11" s="3"/>
       <c r="W11" s="2"/>
@@ -1495,10 +1510,10 @@
       <c r="C12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T12" s="3"/>
       <c r="W12" s="2"/>
@@ -1511,10 +1526,10 @@
       <c r="AL12" s="3"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY12" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="AY12" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="BD12" s="3"/>
       <c r="BF12" s="3"/>
@@ -1523,26 +1538,26 @@
       <c r="C13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="T13" s="3"/>
       <c r="W13" s="2"/>
       <c r="X13" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AL13" s="3"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="AY13" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="BD13" s="3"/>
       <c r="BF13" s="3"/>
@@ -1559,18 +1574,18 @@
       <c r="T14" s="3"/>
       <c r="W14" s="2"/>
       <c r="X14" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AL14" s="3"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AY14" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="AY14" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="BD14" s="3"/>
       <c r="BF14" s="3"/>
@@ -1586,19 +1601,22 @@
       </c>
       <c r="T15" s="3"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="X15" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y15" s="47"/>
+      <c r="Z15" s="47"/>
+      <c r="AA15" s="47"/>
       <c r="AG15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AL15" s="3"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AY15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BD15" s="3"/>
       <c r="BF15" s="3"/>
@@ -1617,10 +1635,10 @@
       <c r="AL16" s="3"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AY16" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="BD16" s="3"/>
       <c r="BF16" s="3"/>
@@ -1629,20 +1647,22 @@
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="T17" s="3"/>
       <c r="W17" s="2"/>
       <c r="AL17" s="3"/>
       <c r="AO17" s="2"/>
-      <c r="AP17" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="AP17" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ17" s="47"/>
+      <c r="AR17" s="47"/>
       <c r="AY17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="BD17" s="3"/>
       <c r="BF17" s="3"/>
@@ -1651,10 +1671,10 @@
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T18" s="3"/>
       <c r="W18" s="2"/>
@@ -1683,10 +1703,10 @@
       <c r="C20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="T20" s="3"/>
       <c r="W20" s="2"/>
@@ -1699,10 +1719,10 @@
       <c r="C21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="T21" s="3"/>
       <c r="W21" s="2"/>
@@ -1808,92 +1828,92 @@
     <row r="26" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="E26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AO26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP26" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="AP26" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="BF26" s="3"/>
     </row>
     <row r="27" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
       <c r="E27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AP27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BF27" s="3"/>
     </row>
     <row r="28" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C28" s="2"/>
       <c r="E28" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F28" s="40" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AO28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AP28" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BF28" s="3"/>
     </row>
     <row r="29" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C29" s="2"/>
       <c r="F29" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="W29" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="X29" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="W29" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="X29" s="42" t="s">
-        <v>96</v>
-      </c>
       <c r="AO29" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AP29" s="42" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BF29" s="3"/>
     </row>
     <row r="30" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="E30" s="39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F30" s="40" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="X30" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AP30" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BF30" s="3"/>
     </row>
@@ -1911,7 +1931,7 @@
     <row r="33" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C33" s="2"/>
       <c r="E33" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
@@ -1929,7 +1949,7 @@
       <c r="S33" s="13"/>
       <c r="T33" s="14"/>
       <c r="W33" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
@@ -1947,7 +1967,7 @@
       <c r="AK33" s="13"/>
       <c r="AL33" s="14"/>
       <c r="AO33" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP33" s="40"/>
       <c r="AQ33" s="40"/>
@@ -1961,7 +1981,7 @@
       <c r="AL34" s="3"/>
       <c r="AO34" s="40"/>
       <c r="AP34" s="41" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AQ34" s="40"/>
       <c r="BF34" s="3"/>
@@ -1970,7 +1990,7 @@
       <c r="C35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
@@ -1981,7 +2001,7 @@
       <c r="M35" s="32"/>
       <c r="N35" s="32"/>
       <c r="O35" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P35" s="32"/>
       <c r="Q35" s="32"/>
@@ -1990,7 +2010,7 @@
       <c r="T35" s="29"/>
       <c r="W35" s="24"/>
       <c r="X35" s="35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y35" s="35"/>
       <c r="Z35" s="35"/>
@@ -2001,7 +2021,7 @@
       <c r="AE35" s="35"/>
       <c r="AF35" s="35"/>
       <c r="AG35" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AH35" s="35"/>
       <c r="AI35" s="35"/>
@@ -2010,7 +2030,7 @@
       <c r="AL35" s="36"/>
       <c r="AO35" s="40"/>
       <c r="AP35" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AQ35" s="40"/>
       <c r="BF35" s="3"/>
@@ -2023,7 +2043,7 @@
       <c r="AL36" s="3"/>
       <c r="AO36" s="40"/>
       <c r="AP36" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AQ36" s="40"/>
       <c r="BF36" s="3"/>
@@ -2032,23 +2052,23 @@
       <c r="C37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O37" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="T37" s="3"/>
       <c r="W37" s="2"/>
       <c r="X37" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AG37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AL37" s="3"/>
       <c r="AO37" s="40"/>
       <c r="AP37" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AQ37" s="40"/>
       <c r="BF37" s="3"/>
@@ -2057,7 +2077,7 @@
       <c r="C38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
@@ -2068,7 +2088,7 @@
       <c r="M38" s="33"/>
       <c r="N38" s="33"/>
       <c r="O38" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P38" s="33"/>
       <c r="Q38" s="33"/>
@@ -2097,7 +2117,7 @@
       <c r="AL38" s="11"/>
       <c r="AO38" s="40"/>
       <c r="AP38" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="AQ38" s="40"/>
       <c r="BF38" s="3"/>
@@ -2106,7 +2126,7 @@
       <c r="C39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
@@ -2117,7 +2137,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P39" s="16"/>
       <c r="Q39" s="16"/>
@@ -2126,7 +2146,7 @@
       <c r="T39" s="17"/>
       <c r="W39" s="2"/>
       <c r="X39" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y39" s="16"/>
       <c r="Z39" s="16"/>
@@ -2137,7 +2157,7 @@
       <c r="AE39" s="16"/>
       <c r="AF39" s="16"/>
       <c r="AG39" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AH39" s="16"/>
       <c r="AI39" s="16"/>
@@ -2147,7 +2167,7 @@
       <c r="AN39" s="22"/>
       <c r="AO39" s="40"/>
       <c r="AP39" s="43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="AQ39" s="40"/>
       <c r="BF39" s="3"/>
@@ -2156,15 +2176,15 @@
       <c r="C40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="T40" s="3"/>
       <c r="W40" s="2"/>
       <c r="X40" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y40" s="38"/>
       <c r="Z40" s="38"/>
@@ -2175,7 +2195,7 @@
       <c r="AE40" s="38"/>
       <c r="AF40" s="38"/>
       <c r="AG40" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AH40" s="18"/>
       <c r="AI40" s="18"/>
@@ -2192,7 +2212,7 @@
       <c r="T41" s="3"/>
       <c r="W41" s="2"/>
       <c r="X41" s="38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Y41" s="38"/>
       <c r="Z41" s="38"/>
@@ -2203,7 +2223,7 @@
       <c r="AE41" s="38"/>
       <c r="AF41" s="38"/>
       <c r="AG41" s="38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AH41" s="18"/>
       <c r="AI41" s="18"/>
@@ -2211,7 +2231,7 @@
       <c r="AK41" s="18"/>
       <c r="AL41" s="3"/>
       <c r="AP41" s="40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="BF41" s="3"/>
     </row>
@@ -2221,10 +2241,10 @@
       <c r="T42" s="3"/>
       <c r="W42" s="2"/>
       <c r="X42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AG42" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="AG42" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="AL42" s="3"/>
       <c r="BF42" s="3"/>
@@ -2241,10 +2261,10 @@
       <c r="C44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O44" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="T44" s="3"/>
       <c r="W44" s="2"/>
@@ -2308,10 +2328,10 @@
       <c r="G47" s="37"/>
       <c r="H47" s="37"/>
       <c r="W47" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="X47" s="37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="BF47" s="3"/>
     </row>
@@ -2322,17 +2342,17 @@
       <c r="G48" s="37"/>
       <c r="H48" s="37"/>
       <c r="X48" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="BF48" s="3"/>
     </row>
     <row r="49" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C49" s="2"/>
       <c r="W49" s="40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="X49" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BF49" s="3"/>
     </row>
@@ -2340,7 +2360,7 @@
       <c r="C50" s="2"/>
       <c r="W50" s="40"/>
       <c r="X50" s="40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BF50" s="3"/>
     </row>

</xml_diff>

<commit_message>
[user-app] <4> VehicleListPage 작성 계속   - UI 오작동 버그 수정
</commit_message>
<xml_diff>
--- a/0 _ docs/0 _ db 설계.xlsx
+++ b/0 _ docs/0 _ db 설계.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\dev-ezen\rental-cars\0 _ docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15AA1031-992A-43CE-80B5-45DF8D37D534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737B5E17-CACD-4C91-AD50-B74583FF9186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{27D1F9A5-D906-4A19-AD47-54230B13E495}"/>
   </bookViews>
@@ -190,10 +190,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>img</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>이미지</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -486,7 +482,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>DB 설계 (최종 수정: 2024.02.15.THU 12:15:00)</t>
+    <t>v_img</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>DB 설계 (최종 수정: 2024.02.16.FRI 09:45:00)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -882,6 +882,9 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,9 +893,6 @@
     </xf>
     <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1216,8 +1216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98531398-C03B-4527-8006-CCEE9F94C8A2}">
   <dimension ref="C2:BF52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:BF3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -1227,64 +1227,64 @@
   <sheetData>
     <row r="2" spans="3:58" ht="14.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="3:58" ht="26.25" x14ac:dyDescent="0.3">
-      <c r="C3" s="44" t="s">
+      <c r="C3" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="45"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="45"/>
-      <c r="AA3" s="45"/>
-      <c r="AB3" s="45"/>
-      <c r="AC3" s="45"/>
-      <c r="AD3" s="45"/>
-      <c r="AE3" s="45"/>
-      <c r="AF3" s="45"/>
-      <c r="AG3" s="45"/>
-      <c r="AH3" s="45"/>
-      <c r="AI3" s="45"/>
-      <c r="AJ3" s="45"/>
-      <c r="AK3" s="45"/>
-      <c r="AL3" s="45"/>
-      <c r="AM3" s="45"/>
-      <c r="AN3" s="45"/>
-      <c r="AO3" s="45"/>
-      <c r="AP3" s="45"/>
-      <c r="AQ3" s="45"/>
-      <c r="AR3" s="45"/>
-      <c r="AS3" s="45"/>
-      <c r="AT3" s="45"/>
-      <c r="AU3" s="45"/>
-      <c r="AV3" s="45"/>
-      <c r="AW3" s="45"/>
-      <c r="AX3" s="45"/>
-      <c r="AY3" s="45"/>
-      <c r="AZ3" s="45"/>
-      <c r="BA3" s="45"/>
-      <c r="BB3" s="45"/>
-      <c r="BC3" s="45"/>
-      <c r="BD3" s="45"/>
-      <c r="BE3" s="45"/>
-      <c r="BF3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="46"/>
+      <c r="AE3" s="46"/>
+      <c r="AF3" s="46"/>
+      <c r="AG3" s="46"/>
+      <c r="AH3" s="46"/>
+      <c r="AI3" s="46"/>
+      <c r="AJ3" s="46"/>
+      <c r="AK3" s="46"/>
+      <c r="AL3" s="46"/>
+      <c r="AM3" s="46"/>
+      <c r="AN3" s="46"/>
+      <c r="AO3" s="46"/>
+      <c r="AP3" s="46"/>
+      <c r="AQ3" s="46"/>
+      <c r="AR3" s="46"/>
+      <c r="AS3" s="46"/>
+      <c r="AT3" s="46"/>
+      <c r="AU3" s="46"/>
+      <c r="AV3" s="46"/>
+      <c r="AW3" s="46"/>
+      <c r="AX3" s="46"/>
+      <c r="AY3" s="46"/>
+      <c r="AZ3" s="46"/>
+      <c r="BA3" s="46"/>
+      <c r="BB3" s="46"/>
+      <c r="BC3" s="46"/>
+      <c r="BD3" s="46"/>
+      <c r="BE3" s="46"/>
+      <c r="BF3" s="47"/>
     </row>
     <row r="4" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
@@ -1333,7 +1333,7 @@
       <c r="AK6" s="13"/>
       <c r="AL6" s="14"/>
       <c r="AO6" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AP6" s="13"/>
       <c r="AQ6" s="13"/>
@@ -1406,7 +1406,7 @@
       <c r="AL8" s="21"/>
       <c r="AO8" s="24"/>
       <c r="AP8" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AQ8" s="27"/>
       <c r="AR8" s="27"/>
@@ -1482,10 +1482,10 @@
       <c r="C11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O11" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="T11" s="3"/>
       <c r="W11" s="2"/>
@@ -1510,10 +1510,10 @@
       <c r="C12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T12" s="3"/>
       <c r="W12" s="2"/>
@@ -1525,11 +1525,13 @@
       </c>
       <c r="AL12" s="3"/>
       <c r="AO12" s="2"/>
-      <c r="AP12" s="1" t="s">
+      <c r="AP12" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="AQ12" s="44"/>
+      <c r="AR12" s="44"/>
+      <c r="AY12" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="AY12" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="BD12" s="3"/>
       <c r="BF12" s="3"/>
@@ -1538,10 +1540,10 @@
       <c r="C13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="T13" s="3"/>
       <c r="W13" s="2"/>
@@ -1601,22 +1603,22 @@
       </c>
       <c r="T15" s="3"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="Y15" s="47"/>
-      <c r="Z15" s="47"/>
-      <c r="AA15" s="47"/>
+      <c r="X15" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y15" s="44"/>
+      <c r="Z15" s="44"/>
+      <c r="AA15" s="44"/>
       <c r="AG15" s="1" t="s">
         <v>22</v>
       </c>
       <c r="AL15" s="3"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AY15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="BD15" s="3"/>
       <c r="BF15" s="3"/>
@@ -1635,10 +1637,10 @@
       <c r="AL16" s="3"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AY16" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BD16" s="3"/>
       <c r="BF16" s="3"/>
@@ -1647,20 +1649,20 @@
       <c r="C17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="T17" s="3"/>
       <c r="W17" s="2"/>
       <c r="AL17" s="3"/>
       <c r="AO17" s="2"/>
-      <c r="AP17" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="AQ17" s="47"/>
-      <c r="AR17" s="47"/>
+      <c r="AP17" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ17" s="44"/>
+      <c r="AR17" s="44"/>
       <c r="AY17" s="1" t="s">
         <v>22</v>
       </c>
@@ -1671,10 +1673,10 @@
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="T18" s="3"/>
       <c r="W18" s="2"/>
@@ -1703,10 +1705,10 @@
       <c r="C20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="T20" s="3"/>
       <c r="W20" s="2"/>
@@ -1719,10 +1721,10 @@
       <c r="C21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O21" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="T21" s="3"/>
       <c r="W21" s="2"/>
@@ -1831,89 +1833,89 @@
         <v>29</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W26" s="1" t="s">
         <v>29</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AO26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP26" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="AP26" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="BF26" s="3"/>
     </row>
     <row r="27" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C27" s="2"/>
       <c r="E27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AP27" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="BF27" s="3"/>
     </row>
     <row r="28" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C28" s="2"/>
       <c r="E28" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F28" s="40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AO28" s="1" t="s">
         <v>29</v>
       </c>
       <c r="AP28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BF28" s="3"/>
     </row>
     <row r="29" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C29" s="2"/>
       <c r="F29" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="W29" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="X29" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="W29" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="X29" s="42" t="s">
-        <v>95</v>
-      </c>
       <c r="AO29" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AP29" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="BF29" s="3"/>
     </row>
     <row r="30" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C30" s="2"/>
       <c r="E30" s="39" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F30" s="40" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X30" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AP30" s="42" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="BF30" s="3"/>
     </row>
@@ -1931,7 +1933,7 @@
     <row r="33" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C33" s="2"/>
       <c r="E33" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
@@ -1967,7 +1969,7 @@
       <c r="AK33" s="13"/>
       <c r="AL33" s="14"/>
       <c r="AO33" s="38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AP33" s="40"/>
       <c r="AQ33" s="40"/>
@@ -1981,7 +1983,7 @@
       <c r="AL34" s="3"/>
       <c r="AO34" s="40"/>
       <c r="AP34" s="41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AQ34" s="40"/>
       <c r="BF34" s="3"/>
@@ -1990,7 +1992,7 @@
       <c r="C35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
@@ -2001,7 +2003,7 @@
       <c r="M35" s="32"/>
       <c r="N35" s="32"/>
       <c r="O35" s="32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P35" s="32"/>
       <c r="Q35" s="32"/>
@@ -2030,7 +2032,7 @@
       <c r="AL35" s="36"/>
       <c r="AO35" s="40"/>
       <c r="AP35" s="40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AQ35" s="40"/>
       <c r="BF35" s="3"/>
@@ -2043,7 +2045,7 @@
       <c r="AL36" s="3"/>
       <c r="AO36" s="40"/>
       <c r="AP36" s="40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AQ36" s="40"/>
       <c r="BF36" s="3"/>
@@ -2052,23 +2054,23 @@
       <c r="C37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="O37" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="T37" s="3"/>
       <c r="W37" s="2"/>
       <c r="X37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AG37" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AL37" s="3"/>
       <c r="AO37" s="40"/>
       <c r="AP37" s="40" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="AQ37" s="40"/>
       <c r="BF37" s="3"/>
@@ -2077,7 +2079,7 @@
       <c r="C38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="34" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
@@ -2088,7 +2090,7 @@
       <c r="M38" s="33"/>
       <c r="N38" s="33"/>
       <c r="O38" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P38" s="33"/>
       <c r="Q38" s="33"/>
@@ -2117,7 +2119,7 @@
       <c r="AL38" s="11"/>
       <c r="AO38" s="40"/>
       <c r="AP38" s="40" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="AQ38" s="40"/>
       <c r="BF38" s="3"/>
@@ -2126,7 +2128,7 @@
       <c r="C39" s="2"/>
       <c r="E39" s="2"/>
       <c r="F39" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G39" s="16"/>
       <c r="H39" s="16"/>
@@ -2137,7 +2139,7 @@
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P39" s="16"/>
       <c r="Q39" s="16"/>
@@ -2146,7 +2148,7 @@
       <c r="T39" s="17"/>
       <c r="W39" s="2"/>
       <c r="X39" s="23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Y39" s="16"/>
       <c r="Z39" s="16"/>
@@ -2157,7 +2159,7 @@
       <c r="AE39" s="16"/>
       <c r="AF39" s="16"/>
       <c r="AG39" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AH39" s="16"/>
       <c r="AI39" s="16"/>
@@ -2167,7 +2169,7 @@
       <c r="AN39" s="22"/>
       <c r="AO39" s="40"/>
       <c r="AP39" s="43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AQ39" s="40"/>
       <c r="BF39" s="3"/>
@@ -2176,15 +2178,15 @@
       <c r="C40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O40" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="T40" s="3"/>
       <c r="W40" s="2"/>
       <c r="X40" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y40" s="38"/>
       <c r="Z40" s="38"/>
@@ -2195,7 +2197,7 @@
       <c r="AE40" s="38"/>
       <c r="AF40" s="38"/>
       <c r="AG40" s="38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="AH40" s="18"/>
       <c r="AI40" s="18"/>
@@ -2212,7 +2214,7 @@
       <c r="T41" s="3"/>
       <c r="W41" s="2"/>
       <c r="X41" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="Y41" s="38"/>
       <c r="Z41" s="38"/>
@@ -2223,7 +2225,7 @@
       <c r="AE41" s="38"/>
       <c r="AF41" s="38"/>
       <c r="AG41" s="38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AH41" s="18"/>
       <c r="AI41" s="18"/>
@@ -2231,7 +2233,7 @@
       <c r="AK41" s="18"/>
       <c r="AL41" s="3"/>
       <c r="AP41" s="40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="BF41" s="3"/>
     </row>
@@ -2241,10 +2243,10 @@
       <c r="T42" s="3"/>
       <c r="W42" s="2"/>
       <c r="X42" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG42" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="AG42" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="AL42" s="3"/>
       <c r="BF42" s="3"/>
@@ -2261,10 +2263,10 @@
       <c r="C44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="O44" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="T44" s="3"/>
       <c r="W44" s="2"/>
@@ -2331,7 +2333,7 @@
         <v>29</v>
       </c>
       <c r="X47" s="37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="BF47" s="3"/>
     </row>
@@ -2342,17 +2344,17 @@
       <c r="G48" s="37"/>
       <c r="H48" s="37"/>
       <c r="X48" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BF48" s="3"/>
     </row>
     <row r="49" spans="3:58" x14ac:dyDescent="0.3">
       <c r="C49" s="2"/>
       <c r="W49" s="40" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X49" s="40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BF49" s="3"/>
     </row>
@@ -2360,7 +2362,7 @@
       <c r="C50" s="2"/>
       <c r="W50" s="40"/>
       <c r="X50" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BF50" s="3"/>
     </row>

</xml_diff>